<commit_message>
2022.5.23 add actions:Yuki,Anna , Quick Method to unzip animations
</commit_message>
<xml_diff>
--- a/tmp/.character .xlsx
+++ b/tmp/.character .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yupooooo\SchoolWork\110-2\ObjectOrientedProgram Lab\Re-Dive\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F01AD7-F31E-488D-88A9-2BDCA521C343}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32F2B87-B282-4006-9496-CE30EBA2C89D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9750" yWindow="1485" windowWidth="10170" windowHeight="1530" xr2:uid="{42B7F6A8-C0B4-450C-914A-32C598DE96A4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Pecorine</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -170,6 +170,10 @@
   </si>
   <si>
     <t>Akari</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -545,7 +549,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -623,6 +627,9 @@
       <c r="B7" t="s">
         <v>6</v>
       </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -630,6 +637,9 @@
       </c>
       <c r="B8" t="s">
         <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
2022.5.23 update Actions :unfinished to 1020 Mimi
</commit_message>
<xml_diff>
--- a/tmp/.character .xlsx
+++ b/tmp/.character .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yupooooo\SchoolWork\110-2\ObjectOrientedProgram Lab\Re-Dive\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32F2B87-B282-4006-9496-CE30EBA2C89D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0CA372-4BC4-43C3-BED8-A6B858CDA2CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9750" yWindow="1485" windowWidth="10170" windowHeight="1530" xr2:uid="{42B7F6A8-C0B4-450C-914A-32C598DE96A4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>Pecorine</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -182,6 +182,10 @@
   </si>
   <si>
     <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -548,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653F9496-248B-4CC0-B791-9C9BBD47807A}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -649,6 +653,9 @@
       <c r="B9" t="s">
         <v>8</v>
       </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -657,6 +664,9 @@
       <c r="B10" t="s">
         <v>9</v>
       </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -665,6 +675,9 @@
       <c r="B11" t="s">
         <v>10</v>
       </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -673,6 +686,9 @@
       <c r="B12" t="s">
         <v>11</v>
       </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -681,6 +697,9 @@
       <c r="B13" t="s">
         <v>12</v>
       </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -689,6 +708,9 @@
       <c r="B14" t="s">
         <v>13</v>
       </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -696,6 +718,9 @@
       </c>
       <c r="B15" t="s">
         <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
2022.5.24 add actions:all charaters completed!
</commit_message>
<xml_diff>
--- a/tmp/.character .xlsx
+++ b/tmp/.character .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yupooooo\SchoolWork\110-2\ObjectOrientedProgram Lab\Re-Dive\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0CA372-4BC4-43C3-BED8-A6B858CDA2CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329D32CA-0409-4AEB-AEEF-EAB0A2AC0BA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9750" yWindow="1485" windowWidth="10170" windowHeight="1530" xr2:uid="{42B7F6A8-C0B4-450C-914A-32C598DE96A4}"/>
+    <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11235" xr2:uid="{42B7F6A8-C0B4-450C-914A-32C598DE96A4}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
   <si>
     <t>Pecorine</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,94 +98,121 @@
     <t>Ninon</t>
   </si>
   <si>
+    <t>Akino</t>
+  </si>
+  <si>
+    <t>Mahiru</t>
+  </si>
+  <si>
+    <t>Shiori</t>
+  </si>
+  <si>
+    <t>Aoi</t>
+  </si>
+  <si>
+    <t>Makoto</t>
+  </si>
+  <si>
+    <t>Kuuka</t>
+  </si>
+  <si>
+    <t>Tamaki</t>
+  </si>
+  <si>
+    <t>Mifuyu</t>
+  </si>
+  <si>
+    <t>Shizuru</t>
+  </si>
+  <si>
+    <t>Mitsuki</t>
+  </si>
+  <si>
+    <t>Rima</t>
+  </si>
+  <si>
+    <t>Monika</t>
+  </si>
+  <si>
+    <t>Djeeta</t>
+  </si>
+  <si>
+    <t>Chika</t>
+  </si>
+  <si>
+    <t>Arisa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yui</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Misogi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Akari</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Shinobu</t>
-  </si>
-  <si>
-    <t>Akino</t>
-  </si>
-  <si>
-    <t>Mahiru</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Yukari</t>
-  </si>
-  <si>
-    <t>Shiori</t>
-  </si>
-  <si>
-    <t>Aoi</t>
-  </si>
-  <si>
-    <t>Makoto</t>
-  </si>
-  <si>
-    <t>Kuuka</t>
-  </si>
-  <si>
-    <t>Tamaki</t>
-  </si>
-  <si>
-    <t>Mifuyu</t>
-  </si>
-  <si>
-    <t>Shizuru</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>63 56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Misaki</t>
-  </si>
-  <si>
-    <t>Mitsuki</t>
-  </si>
-  <si>
-    <t>Rima</t>
-  </si>
-  <si>
-    <t>Monika</t>
-  </si>
-  <si>
-    <t>Djeeta</t>
-  </si>
-  <si>
-    <t>Chika</t>
-  </si>
-  <si>
-    <t>Arisa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yui</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Misogi</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Akari</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill1 broken</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill0 problem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>warn: skill0 超大</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -550,13 +577,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653F9496-248B-4CC0-B791-9C9BBD47807A}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="18.125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -566,7 +596,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -574,10 +604,10 @@
         <v>1002</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -588,7 +618,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -596,10 +626,10 @@
         <v>1004</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -607,10 +637,10 @@
         <v>1006</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -621,7 +651,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -632,7 +662,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -643,7 +673,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -654,7 +684,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -665,7 +695,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -676,7 +706,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -687,7 +717,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -698,7 +728,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -709,7 +739,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -720,7 +750,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -730,192 +760,273 @@
       <c r="B16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1022</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1025</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1027</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1028</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1029</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1030</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1031</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1032</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1033</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1034</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1038</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="C27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1040</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1042</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1043</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1045</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1046</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="C32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1048</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1049</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1050</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="C35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1051</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1052</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="C37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1053</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="C38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1057</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="C39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1058</v>
       </c>
@@ -923,10 +1034,10 @@
         <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1059</v>
       </c>
@@ -934,10 +1045,10 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1060</v>
       </c>
@@ -945,18 +1056,23 @@
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1063</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C43" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2022/05/26 Add all character class
</commit_message>
<xml_diff>
--- a/tmp/.character .xlsx
+++ b/tmp/.character .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yupooooo\SchoolWork\110-2\ObjectOrientedProgram Lab\Re-Dive\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Homework\PrincessConnectReDive\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329D32CA-0409-4AEB-AEEF-EAB0A2AC0BA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8541A113-BF2C-4DE8-BDC4-3309FF8E27A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11235" xr2:uid="{42B7F6A8-C0B4-450C-914A-32C598DE96A4}"/>
+    <workbookView xWindow="10452" yWindow="1680" windowWidth="10164" windowHeight="8184" xr2:uid="{42B7F6A8-C0B4-450C-914A-32C598DE96A4}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="54">
   <si>
     <t>Pecorine</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,172 +47,194 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Shizuru</t>
+  </si>
+  <si>
+    <t>Mitsuki</t>
+  </si>
+  <si>
+    <t>Rima</t>
+  </si>
+  <si>
+    <t>Monika</t>
+  </si>
+  <si>
+    <t>Djeeta</t>
+  </si>
+  <si>
+    <t>Arisa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yui</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Misogi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Akari</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shinobu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yukari</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>63 56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Misaki</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill1 broken</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>warn: skill0 超大</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Miyako</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Yuki</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Anna</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Maho</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Rino</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Hatsune</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Suzuna</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Kaori</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Io</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Mimi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Kurumi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Yori</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Suzume</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Eriko</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Saren</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Nozomi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ninon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Akino</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Mahiru</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Shiori</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Aoi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chika</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Makoto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Kuuka</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Tamaki</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Mifuyu</t>
-  </si>
-  <si>
-    <t>Shizuru</t>
-  </si>
-  <si>
-    <t>Mitsuki</t>
-  </si>
-  <si>
-    <t>Rima</t>
-  </si>
-  <si>
-    <t>Monika</t>
-  </si>
-  <si>
-    <t>Djeeta</t>
-  </si>
-  <si>
-    <t>Chika</t>
-  </si>
-  <si>
-    <t>Arisa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yui</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Misogi</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Akari</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shinobu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yukari</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>63 56</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Misaki</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill1 broken</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>skill0 problem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>warn: skill0 超大</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -579,16 +601,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653F9496-248B-4CC0-B791-9C9BBD47807A}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="18.125" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1001</v>
       </c>
@@ -596,21 +618,21 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1002</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1003</v>
       </c>
@@ -618,415 +640,412 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1004</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1006</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1007</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1008</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1009</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1010</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1011</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1012</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1016</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1017</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1018</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1020</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1021</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1022</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1025</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1027</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1028</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1029</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1030</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1031</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1032</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1033</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1034</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1038</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1040</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1042</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1043</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1045</v>
       </c>
       <c r="B31" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1046</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1048</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1049</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1050</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1051</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1052</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1053</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D38" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1057</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1058</v>
       </c>
@@ -1034,10 +1053,10 @@
         <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1059</v>
       </c>
@@ -1045,10 +1064,10 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1060</v>
       </c>
@@ -1056,23 +1075,23 @@
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1063</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C43" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>